<commit_message>
Updated project with latest fixes and features
</commit_message>
<xml_diff>
--- a/app/static/reports/technician_foc_warranty_report.xlsx
+++ b/app/static/reports/technician_foc_warranty_report.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F33"/>
+  <dimension ref="A1:F34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -472,19 +472,19 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="C2" t="n">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="D2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E2" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F2" t="n">
-        <v>11</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3">
@@ -494,19 +494,19 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="C3" t="n">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="D3" t="n">
         <v>0</v>
       </c>
       <c r="E3" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="F3" t="n">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4">
@@ -516,19 +516,19 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C4" t="n">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="D4" t="n">
         <v>0</v>
       </c>
       <c r="E4" t="n">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="F4" t="n">
-        <v>7</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5">
@@ -538,19 +538,19 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C5" t="n">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="D5" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E5" t="n">
         <v>0</v>
       </c>
       <c r="F5" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6">
@@ -560,10 +560,10 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="C6" t="n">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="D6" t="n">
         <v>0</v>
@@ -572,7 +572,7 @@
         <v>2</v>
       </c>
       <c r="F6" t="n">
-        <v>21</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7">
@@ -582,19 +582,19 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C7" t="n">
-        <v>1</v>
+        <v>26</v>
       </c>
       <c r="D7" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E7" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F7" t="n">
-        <v>15</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8">
@@ -607,16 +607,16 @@
         <v>0</v>
       </c>
       <c r="C8" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D8" t="n">
         <v>1</v>
       </c>
       <c r="E8" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="F8" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9">
@@ -626,19 +626,19 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="C9" t="n">
-        <v>1</v>
+        <v>35</v>
       </c>
       <c r="D9" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E9" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F9" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10">
@@ -648,19 +648,19 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="C10" t="n">
-        <v>1</v>
+        <v>45</v>
       </c>
       <c r="D10" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E10" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F10" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11">
@@ -670,19 +670,19 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C11" t="n">
-        <v>3</v>
+        <v>19</v>
       </c>
       <c r="D11" t="n">
         <v>0</v>
       </c>
       <c r="E11" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="F11" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="12">
@@ -692,19 +692,19 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="C12" t="n">
-        <v>1</v>
+        <v>33</v>
       </c>
       <c r="D12" t="n">
         <v>1</v>
       </c>
       <c r="E12" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F12" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="13">
@@ -714,19 +714,19 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="C13" t="n">
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="D13" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E13" t="n">
         <v>2</v>
       </c>
       <c r="F13" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="14">
@@ -736,19 +736,19 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="C14" t="n">
+        <v>31</v>
+      </c>
+      <c r="D14" t="n">
         <v>2</v>
       </c>
-      <c r="D14" t="n">
-        <v>0</v>
-      </c>
       <c r="E14" t="n">
         <v>1</v>
       </c>
       <c r="F14" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="15">
@@ -761,16 +761,16 @@
         <v>0</v>
       </c>
       <c r="C15" t="n">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="D15" t="n">
         <v>0</v>
       </c>
       <c r="E15" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="F15" t="n">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="16">
@@ -802,10 +802,10 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C17" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="D17" t="n">
         <v>0</v>
@@ -814,7 +814,7 @@
         <v>0</v>
       </c>
       <c r="F17" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18">
@@ -824,19 +824,19 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C18" t="n">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="D18" t="n">
         <v>0</v>
       </c>
       <c r="E18" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F18" t="n">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="19">
@@ -846,16 +846,16 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="C19" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D19" t="n">
         <v>0</v>
       </c>
       <c r="E19" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F19" t="n">
         <v>3</v>
@@ -868,10 +868,10 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C20" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D20" t="n">
         <v>0</v>
@@ -890,19 +890,19 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="C21" t="n">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="D21" t="n">
         <v>0</v>
       </c>
       <c r="E21" t="n">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="F21" t="n">
-        <v>0</v>
+        <v>15</v>
       </c>
     </row>
     <row r="22">
@@ -937,7 +937,7 @@
         <v>0</v>
       </c>
       <c r="C23" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="D23" t="n">
         <v>0</v>
@@ -946,7 +946,7 @@
         <v>1</v>
       </c>
       <c r="F23" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="24">
@@ -978,10 +978,10 @@
         </is>
       </c>
       <c r="B25" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="C25" t="n">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="D25" t="n">
         <v>0</v>
@@ -990,7 +990,7 @@
         <v>1</v>
       </c>
       <c r="F25" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="26">
@@ -1000,10 +1000,10 @@
         </is>
       </c>
       <c r="B26" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="C26" t="n">
-        <v>0</v>
+        <v>36</v>
       </c>
       <c r="D26" t="n">
         <v>0</v>
@@ -1022,10 +1022,10 @@
         </is>
       </c>
       <c r="B27" t="n">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="C27" t="n">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="D27" t="n">
         <v>0</v>
@@ -1047,7 +1047,7 @@
         <v>0</v>
       </c>
       <c r="C28" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D28" t="n">
         <v>0</v>
@@ -1066,10 +1066,10 @@
         </is>
       </c>
       <c r="B29" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C29" t="n">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="D29" t="n">
         <v>0</v>
@@ -1091,7 +1091,7 @@
         <v>0</v>
       </c>
       <c r="C30" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D30" t="n">
         <v>0</v>
@@ -1113,7 +1113,7 @@
         <v>0</v>
       </c>
       <c r="C31" t="n">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="D31" t="n">
         <v>0</v>
@@ -1122,7 +1122,7 @@
         <v>0</v>
       </c>
       <c r="F31" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="32">
@@ -1150,22 +1150,44 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>SAIFAR ABDUL LATHEEF</t>
+          <t>Bbaale  Jean</t>
         </is>
       </c>
       <c r="B33" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C33" t="n">
-        <v>4</v>
+        <v>26</v>
       </c>
       <c r="D33" t="n">
         <v>0</v>
       </c>
       <c r="E33" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F33" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>Boas Massinde</t>
+        </is>
+      </c>
+      <c r="B34" t="n">
+        <v>0</v>
+      </c>
+      <c r="C34" t="n">
+        <v>0</v>
+      </c>
+      <c r="D34" t="n">
+        <v>0</v>
+      </c>
+      <c r="E34" t="n">
+        <v>0</v>
+      </c>
+      <c r="F34" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated about.html with watermark and improved layout
</commit_message>
<xml_diff>
--- a/app/static/reports/technician_foc_warranty_report.xlsx
+++ b/app/static/reports/technician_foc_warranty_report.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F34"/>
+  <dimension ref="A1:F33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -472,7 +472,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C2" t="n">
         <v>18</v>
@@ -484,7 +484,7 @@
         <v>3</v>
       </c>
       <c r="F2" t="n">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3">
@@ -494,19 +494,19 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C3" t="n">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D3" t="n">
         <v>0</v>
       </c>
       <c r="E3" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="F3" t="n">
-        <v>11</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4">
@@ -516,10 +516,10 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C4" t="n">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="D4" t="n">
         <v>0</v>
@@ -528,7 +528,7 @@
         <v>15</v>
       </c>
       <c r="F4" t="n">
-        <v>13</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5">
@@ -541,7 +541,7 @@
         <v>1</v>
       </c>
       <c r="C5" t="n">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D5" t="n">
         <v>0</v>
@@ -563,7 +563,7 @@
         <v>5</v>
       </c>
       <c r="C6" t="n">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D6" t="n">
         <v>0</v>
@@ -572,7 +572,7 @@
         <v>2</v>
       </c>
       <c r="F6" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7">
@@ -585,10 +585,10 @@
         <v>2</v>
       </c>
       <c r="C7" t="n">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="D7" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E7" t="n">
         <v>1</v>
@@ -626,19 +626,19 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C9" t="n">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="D9" t="n">
         <v>3</v>
       </c>
       <c r="E9" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F9" t="n">
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10">
@@ -648,19 +648,19 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C10" t="n">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="D10" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E10" t="n">
         <v>2</v>
       </c>
       <c r="F10" t="n">
-        <v>1</v>
+        <v>16</v>
       </c>
     </row>
     <row r="11">
@@ -670,16 +670,16 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C11" t="n">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D11" t="n">
         <v>0</v>
       </c>
       <c r="E11" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F11" t="n">
         <v>7</v>
@@ -692,19 +692,19 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C12" t="n">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="D12" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E12" t="n">
         <v>4</v>
       </c>
       <c r="F12" t="n">
-        <v>8</v>
+        <v>13</v>
       </c>
     </row>
     <row r="13">
@@ -714,10 +714,10 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C13" t="n">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="D13" t="n">
         <v>3</v>
@@ -726,7 +726,7 @@
         <v>2</v>
       </c>
       <c r="F13" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14">
@@ -736,10 +736,10 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C14" t="n">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="D14" t="n">
         <v>2</v>
@@ -758,7 +758,7 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C15" t="n">
         <v>21</v>
@@ -770,7 +770,7 @@
         <v>0</v>
       </c>
       <c r="F15" t="n">
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
     <row r="16">
@@ -805,7 +805,7 @@
         <v>3</v>
       </c>
       <c r="C17" t="n">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="D17" t="n">
         <v>0</v>
@@ -824,7 +824,7 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C18" t="n">
         <v>21</v>
@@ -836,7 +836,7 @@
         <v>1</v>
       </c>
       <c r="F18" t="n">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="19">
@@ -849,7 +849,7 @@
         <v>7</v>
       </c>
       <c r="C19" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="D19" t="n">
         <v>0</v>
@@ -858,7 +858,7 @@
         <v>3</v>
       </c>
       <c r="F19" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20">
@@ -868,10 +868,10 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C20" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D20" t="n">
         <v>0</v>
@@ -893,7 +893,7 @@
         <v>6</v>
       </c>
       <c r="C21" t="n">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D21" t="n">
         <v>0</v>
@@ -902,7 +902,7 @@
         <v>17</v>
       </c>
       <c r="F21" t="n">
-        <v>15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22">
@@ -934,7 +934,7 @@
         </is>
       </c>
       <c r="B23" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C23" t="n">
         <v>10</v>
@@ -943,67 +943,67 @@
         <v>0</v>
       </c>
       <c r="E23" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F23" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>NAKIMERA NASHIM</t>
+          <t>Musasizi Eric John</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="C24" t="n">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="D24" t="n">
         <v>0</v>
       </c>
       <c r="E24" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F24" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Musasizi Eric John</t>
+          <t>Muyanja Moses</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C25" t="n">
-        <v>19</v>
+        <v>38</v>
       </c>
       <c r="D25" t="n">
         <v>0</v>
       </c>
       <c r="E25" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F25" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Muyanja Moses</t>
+          <t>MBAZIIRA HUDHAIFA</t>
         </is>
       </c>
       <c r="B26" t="n">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="C26" t="n">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="D26" t="n">
         <v>0</v>
@@ -1018,14 +1018,14 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>MBAZIIRA HUDHAIFA</t>
+          <t>KIWANDA PETER</t>
         </is>
       </c>
       <c r="B27" t="n">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="C27" t="n">
-        <v>27</v>
+        <v>2</v>
       </c>
       <c r="D27" t="n">
         <v>0</v>
@@ -1034,20 +1034,20 @@
         <v>0</v>
       </c>
       <c r="F27" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>KIWANDA PETER</t>
+          <t>Daphine Nakanwagi</t>
         </is>
       </c>
       <c r="B28" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C28" t="n">
-        <v>2</v>
+        <v>26</v>
       </c>
       <c r="D28" t="n">
         <v>0</v>
@@ -1056,20 +1056,20 @@
         <v>0</v>
       </c>
       <c r="F28" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Daphine Nakanwagi</t>
+          <t>Lubega Mark</t>
         </is>
       </c>
       <c r="B29" t="n">
+        <v>2</v>
+      </c>
+      <c r="C29" t="n">
         <v>4</v>
-      </c>
-      <c r="C29" t="n">
-        <v>25</v>
       </c>
       <c r="D29" t="n">
         <v>0</v>
@@ -1084,14 +1084,14 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Lubega Mark</t>
+          <t>Talemwa Steven</t>
         </is>
       </c>
       <c r="B30" t="n">
         <v>0</v>
       </c>
       <c r="C30" t="n">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="D30" t="n">
         <v>0</v>
@@ -1106,14 +1106,14 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Talemwa Steven</t>
+          <t>other</t>
         </is>
       </c>
       <c r="B31" t="n">
         <v>0</v>
       </c>
       <c r="C31" t="n">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="D31" t="n">
         <v>0</v>
@@ -1122,26 +1122,26 @@
         <v>0</v>
       </c>
       <c r="F31" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>Bbaale  Jean</t>
         </is>
       </c>
       <c r="B32" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C32" t="n">
-        <v>0</v>
+        <v>29</v>
       </c>
       <c r="D32" t="n">
         <v>0</v>
       </c>
       <c r="E32" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F32" t="n">
         <v>0</v>
@@ -1150,44 +1150,22 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Bbaale  Jean</t>
+          <t>Boas Massinde</t>
         </is>
       </c>
       <c r="B33" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C33" t="n">
-        <v>26</v>
+        <v>0</v>
       </c>
       <c r="D33" t="n">
         <v>0</v>
       </c>
       <c r="E33" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F33" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" t="inlineStr">
-        <is>
-          <t>Boas Massinde</t>
-        </is>
-      </c>
-      <c r="B34" t="n">
-        <v>0</v>
-      </c>
-      <c r="C34" t="n">
-        <v>0</v>
-      </c>
-      <c r="D34" t="n">
-        <v>0</v>
-      </c>
-      <c r="E34" t="n">
-        <v>0</v>
-      </c>
-      <c r="F34" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>